<commit_message>
Working on navigating to questions
</commit_message>
<xml_diff>
--- a/.00_scratch/lu_info_url_v5_2024-10-11.xlsx
+++ b/.00_scratch/lu_info_url_v5_2024-10-11.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassi\Documents\GitHub_AB-RCSC\rc-decision-support-tool\.00_scratch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABMI_Official\RCDST_Jupyter_webapp_Official\.00_scratch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C5743D8-4312-46B5-895A-0AC9393B02BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35F746B-FF4A-45E4-B123-FEF9886EB19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="690" windowWidth="29040" windowHeight="15720" xr2:uid="{676577D7-ABA9-4DDC-844E-63E7610FB4FE}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{676577D7-ABA9-4DDC-844E-63E7610FB4FE}"/>
   </bookViews>
   <sheets>
     <sheet name="lu_info_url" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,12 +369,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -419,15 +413,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -810,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2777091B-4C64-4389-BCA3-E0DEA649BF94}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,93 +1234,87 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
         <v>98</v>
       </c>
       <c r="B41" t="s">
@@ -1343,7 +1328,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>98</v>
       </c>
       <c r="B42" t="s">
@@ -1426,8 +1411,11 @@
   <hyperlinks>
     <hyperlink ref="D34" r:id="rId1" location="concept-library" xr:uid="{3D849CFD-562B-418D-BEAE-46E4AC66459F}"/>
     <hyperlink ref="D35" r:id="rId2" xr:uid="{2E5C6128-2F04-4E11-87AB-6B03D4E84B93}"/>
+    <hyperlink ref="D36" r:id="rId3" xr:uid="{10D9044B-1E50-44BC-BBAF-5A881BD39B11}"/>
+    <hyperlink ref="D37" r:id="rId4" xr:uid="{ECE798EB-8F4D-434D-859A-ECF99929E4D3}"/>
+    <hyperlink ref="D38" r:id="rId5" xr:uid="{A97FA48E-96CC-4BDB-BED2-B98C0618F1CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>